<commit_message>
15484 polys lines points deleted
to be remapped at OWEB
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
   <si>
     <t>project_id</t>
   </si>
@@ -172,6 +172,9 @@
       </rPr>
       <t xml:space="preserve">We often get these types of files for instream LWD placement; they would be mapped as multiple lines along the stream segments to the best of your ability at the start/stop points of the lines.  Call if you have further questions on this one.</t>
     </r>
+  </si>
+  <si>
+    <t>The map shows 2009 – 2012, but the OWRI page shows the project 2010-2012. Should I leave out the 2009 points?</t>
   </si>
   <si>
     <t>Sweet Ranch Ag Water Quality and Estuary Rearing Habitat Restoration</t>
@@ -232,6 +235,9 @@
       <t xml:space="preserve">Please remove points, lines, polys as this will be remapped back here at OWEB
  </t>
     </r>
+  </si>
+  <si>
+    <t>OK, deleted points, lines polys.</t>
   </si>
   <si>
     <t>Tracy Ranch Juniper Cut</t>
@@ -849,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L3" activeCellId="0" pane="topLeft" sqref="L3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L5" activeCellId="0" pane="topLeft" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1004,8 +1010,11 @@
       <c r="K4" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="75" outlineLevel="0" r="5">
+      <c r="L4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="5">
       <c r="A5" s="5" t="n">
         <v>15484</v>
       </c>
@@ -1013,31 +1022,34 @@
         <v>20120428</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
@@ -1048,16 +1060,16 @@
         <v>20120107</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>26</v>
@@ -1069,10 +1081,10 @@
         <v>26</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="153" outlineLevel="0" r="7">
@@ -1083,31 +1095,31 @@
         <v>20120126</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="8">
@@ -1118,31 +1130,31 @@
         <v>20120168</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I8" s="12" t="n">
         <v>31</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="9">
@@ -1153,31 +1165,31 @@
         <v>20120161</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="10">
@@ -1188,31 +1200,31 @@
         <v>20120197</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I10" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="11">
@@ -1223,31 +1235,31 @@
         <v>20120225</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
@@ -1258,14 +1270,14 @@
         <v>20120232</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>26</v>
@@ -1277,10 +1289,10 @@
         <v>26</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
@@ -1291,14 +1303,14 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>26</v>
@@ -1310,10 +1322,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
@@ -1324,14 +1336,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1343,10 +1355,10 @@
         <v>26</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1357,16 +1369,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1378,10 +1390,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1392,10 +1404,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1404,10 +1416,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1416,7 +1428,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1427,10 +1439,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1439,10 +1451,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1451,7 +1463,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1462,31 +1474,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1497,10 +1509,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1509,10 +1521,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1521,7 +1533,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1532,10 +1544,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1544,10 +1556,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1556,7 +1568,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1567,31 +1579,31 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15079 Ginger comments; tracy ranch fixed
wrong project id
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
   <si>
     <t>project_id</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>poly not found 7/ 18</t>
+  </si>
+  <si>
+    <t>I had made a typo for the project id, this is fixed.</t>
   </si>
   <si>
     <t>Morgan Creek Restoration</t>
@@ -856,7 +859,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L5" activeCellId="0" pane="topLeft" sqref="L5"/>
+      <selection activeCell="J7" activeCellId="0" pane="topLeft" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1086,6 +1089,9 @@
       <c r="K6" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="153" outlineLevel="0" r="7">
       <c r="A7" s="10" t="n">
@@ -1095,31 +1101,31 @@
         <v>20120126</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="8">
@@ -1130,22 +1136,22 @@
         <v>20120168</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I8" s="12" t="n">
         <v>31</v>
@@ -1154,7 +1160,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="9">
@@ -1165,31 +1171,31 @@
         <v>20120161</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="10">
@@ -1200,10 +1206,10 @@
         <v>20120197</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>40</v>
@@ -1212,10 +1218,10 @@
         <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I10" s="12" t="n">
         <v>16</v>
@@ -1224,7 +1230,7 @@
         <v>41</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="11">
@@ -1235,31 +1241,31 @@
         <v>20120225</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
@@ -1270,14 +1276,14 @@
         <v>20120232</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>26</v>
@@ -1289,10 +1295,10 @@
         <v>26</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
@@ -1303,14 +1309,14 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>26</v>
@@ -1322,10 +1328,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
@@ -1336,14 +1342,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1355,10 +1361,10 @@
         <v>26</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1369,16 +1375,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1390,10 +1396,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1404,10 +1410,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1416,10 +1422,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1428,7 +1434,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1439,10 +1445,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1451,10 +1457,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1463,7 +1469,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1474,31 +1480,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1509,10 +1515,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1521,10 +1527,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1533,7 +1539,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1544,10 +1550,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1556,10 +1562,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1568,7 +1574,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1579,31 +1585,31 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15090 redone per gingers comments
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="122">
   <si>
     <t>project_id</t>
   </si>
@@ -293,6 +293,9 @@
       </rPr>
       <t xml:space="preserve">This should be mapped as two points and two lines only (no poly), the instream is one line (with all instream treatments noted in the comments), all the riparian work is another line (following the stream layer and with all riparian treatments combined - since it is riparian, you don't need to include in comment i.e. invasive plant control, tree and vegetation planting).  Also, if you have overlapping activities, you place the feature on top of each other; no need to offset as you have done. </t>
     </r>
+  </si>
+  <si>
+    <t>OK, done.</t>
   </si>
   <si>
     <t>Curry Public Library Stormwater Management</t>
@@ -859,7 +862,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J7" activeCellId="0" pane="topLeft" sqref="J7"/>
+      <selection activeCell="L7" activeCellId="0" pane="topLeft" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1127,6 +1130,9 @@
       <c r="K7" s="11" t="s">
         <v>51</v>
       </c>
+      <c r="L7" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="8">
       <c r="A8" s="12" t="n">
@@ -1136,22 +1142,22 @@
         <v>20120168</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I8" s="12" t="n">
         <v>31</v>
@@ -1160,7 +1166,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="9">
@@ -1171,31 +1177,31 @@
         <v>20120161</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="10">
@@ -1206,10 +1212,10 @@
         <v>20120197</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>40</v>
@@ -1218,10 +1224,10 @@
         <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I10" s="12" t="n">
         <v>16</v>
@@ -1230,7 +1236,7 @@
         <v>41</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="11">
@@ -1241,31 +1247,31 @@
         <v>20120225</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
@@ -1276,14 +1282,14 @@
         <v>20120232</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>26</v>
@@ -1295,10 +1301,10 @@
         <v>26</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
@@ -1309,7 +1315,7 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1328,10 +1334,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
@@ -1342,14 +1348,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1361,10 +1367,10 @@
         <v>26</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1375,16 +1381,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1396,10 +1402,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1410,10 +1416,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1422,10 +1428,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1434,7 +1440,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1445,10 +1451,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1457,10 +1463,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1469,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1480,31 +1486,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1515,10 +1521,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1527,10 +1533,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1539,7 +1545,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1550,10 +1556,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1562,10 +1568,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1574,7 +1580,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1585,31 +1591,31 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15138 point and line deleted
needs to be remapped by OWEB
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
   <si>
     <t>project_id</t>
   </si>
@@ -315,6 +315,9 @@
   <si>
     <t>map respondent turned in only gave bioswale info; because OWRI form indicated a wetland had been established, I would expect them to turn in something with  a polygon of roughly .5 acres included; which they didn't.  I have no idea what showing the creek was to indicate.  Please delete the point and line feature for this grant.  In cases such as these, you can either note you cannot map this (wetland) feature; or contact the GIS coordinator at OWEB about what to do.
 Will need to pull grant at OWEB and map here</t>
+  </si>
+  <si>
+    <t>OK, point and line deleted.</t>
   </si>
   <si>
     <t>Malheur Rush Skeletonweed Containment Project</t>
@@ -861,8 +864,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L7" activeCellId="0" pane="topLeft" sqref="L7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L8" activeCellId="0" pane="topLeft" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1134,7 +1137,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="149.25" outlineLevel="0" r="8">
       <c r="A8" s="12" t="n">
         <v>15138</v>
       </c>
@@ -1167,6 +1170,9 @@
       </c>
       <c r="K8" s="13" t="s">
         <v>58</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="9">
@@ -1177,31 +1183,31 @@
         <v>20120161</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="10">
@@ -1212,10 +1218,10 @@
         <v>20120197</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>40</v>
@@ -1224,10 +1230,10 @@
         <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I10" s="12" t="n">
         <v>16</v>
@@ -1236,7 +1242,7 @@
         <v>41</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="11">
@@ -1247,31 +1253,31 @@
         <v>20120225</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
@@ -1282,14 +1288,14 @@
         <v>20120232</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>26</v>
@@ -1301,10 +1307,10 @@
         <v>26</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
@@ -1315,7 +1321,7 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1334,10 +1340,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
@@ -1348,14 +1354,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1367,10 +1373,10 @@
         <v>26</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1381,16 +1387,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1402,10 +1408,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1416,10 +1422,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1428,10 +1434,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1440,7 +1446,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1451,10 +1457,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1463,10 +1469,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1475,7 +1481,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1486,31 +1492,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1521,10 +1527,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1533,10 +1539,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1545,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1556,10 +1562,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1568,10 +1574,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1580,7 +1586,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1591,31 +1597,31 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15188 Ginger comment; deleted polys
to be remapped by OWEB
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="125">
   <si>
     <t>project_id</t>
   </si>
@@ -360,6 +360,9 @@
     </r>
   </si>
   <si>
+    <t>OK.</t>
+  </si>
+  <si>
     <t>Howard Creek Culvert Removal/Replacement</t>
   </si>
   <si>
@@ -374,6 +377,9 @@
   <si>
     <t>Realize this was hard to figure out from their map but fish passage, especially, and instream work, generally, are never represented as a polygons.  
 The two culvert replacements (one point each) are at the road stream crossings as indicated on those layers and according to the map.  The very brief instream work (.01 mile according to the Project File)is represented as a line near project 1.  Since their map placement doesn't match road stream layers, please delete polys. This will need to be mapped at OWEB</t>
+  </si>
+  <si>
+    <t>OK, deleted polys.</t>
   </si>
   <si>
     <t>Five Creeks Riddle Ranch Phase II</t>
@@ -864,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L8" activeCellId="0" pane="topLeft" sqref="L8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L10" activeCellId="0" pane="topLeft" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1209,8 +1215,11 @@
       <c r="K9" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="165" outlineLevel="0" r="10">
+      <c r="L9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="162.65" outlineLevel="0" r="10">
       <c r="A10" s="12" t="n">
         <v>15188</v>
       </c>
@@ -1218,10 +1227,10 @@
         <v>20120197</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>40</v>
@@ -1230,10 +1239,10 @@
         <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="12" t="n">
         <v>16</v>
@@ -1242,7 +1251,10 @@
         <v>41</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="11">
@@ -1253,31 +1265,31 @@
         <v>20120225</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
@@ -1288,14 +1300,14 @@
         <v>20120232</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>26</v>
@@ -1310,7 +1322,7 @@
         <v>67</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
@@ -1321,7 +1333,7 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1340,10 +1352,10 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
@@ -1354,14 +1366,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1376,7 +1388,7 @@
         <v>67</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1387,16 +1399,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1408,10 +1420,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1422,10 +1434,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1434,10 +1446,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1446,7 +1458,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1457,10 +1469,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1469,10 +1481,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1481,7 +1493,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1492,31 +1504,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1527,10 +1539,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1539,10 +1551,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1551,7 +1563,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1562,10 +1574,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1574,10 +1586,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1586,7 +1598,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1597,22 +1609,22 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
@@ -1621,7 +1633,7 @@
         <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15264 Ginger comment; fence including inkind work
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
   <si>
     <t>project_id</t>
   </si>
@@ -870,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L10" activeCellId="0" pane="topLeft" sqref="L10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L11" activeCellId="0" pane="topLeft" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1291,6 +1291,9 @@
       <c r="K11" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
       <c r="A12" s="12" t="n">

</xml_diff>

<commit_message>
github weird; theres a mystery line
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
   <si>
     <t>project_id</t>
   </si>
@@ -428,6 +428,9 @@
     </r>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>Wooly distaff thistle- 2012</t>
   </si>
   <si>
@@ -436,6 +439,9 @@
   <si>
     <t>These points appear to be misidentified as belonging to project 20120257, ri # 15297 instead of 201020272, 15272
  </t>
+  </si>
+  <si>
+    <t>OK, fixed.</t>
   </si>
   <si>
     <t>Carter Creek Riparian Restoration</t>
@@ -870,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L11" activeCellId="0" pane="topLeft" sqref="L11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L14" activeCellId="0" pane="topLeft" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1327,8 +1333,11 @@
       <c r="K12" s="14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="13">
+      <c r="L12" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="55.2" outlineLevel="0" r="13">
       <c r="A13" s="12" t="n">
         <v>15272</v>
       </c>
@@ -1336,7 +1345,7 @@
         <v>20120272</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1355,13 +1364,16 @@
         <v>26</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="14">
+        <v>90</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="149.25" outlineLevel="0" r="14">
       <c r="A14" s="12" t="n">
         <v>15326</v>
       </c>
@@ -1369,14 +1381,14 @@
         <v>20120284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>26</v>
@@ -1391,7 +1403,10 @@
         <v>67</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="180" outlineLevel="0" r="15">
@@ -1402,16 +1417,16 @@
         <v>20120346</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>26</v>
@@ -1423,10 +1438,10 @@
         <v>26</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
@@ -1437,10 +1452,10 @@
         <v>20120435</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>12</v>
@@ -1449,10 +1464,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I16" s="15" t="n">
         <v>30</v>
@@ -1461,7 +1476,7 @@
         <v>17</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1472,10 +1487,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1484,10 +1499,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1496,7 +1511,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1507,31 +1522,31 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1542,10 +1557,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1554,10 +1569,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1566,7 +1581,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1577,10 +1592,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1589,10 +1604,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1601,7 +1616,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1612,22 +1627,22 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
@@ -1636,7 +1651,7 @@
         <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ginger comment xls, about to figure out mystery line
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
   <si>
     <t>project_id</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Realize the map provided was a case of 'too much detailed information'; in reviewing both the OWRI project and the actual grant file, please remove the points and lines you have entered and digitize as follows:  there should be two features, the first is a line (riparian areas should almost always digitized as lines) following the stream line as can be seen in the aerial imagery per the 'excavated pilot channel' in the respondent map i.e., between the two lines you had previously mapped. The hydroseeding (2008 hydroseeding 1.5 acres)should be represented as a polygon, following the outline indicated in the respondent's map.</t>
+  </si>
+  <si>
+    <t>Hydroseeding wasn't in the OWRI page, so I wasn't sure what to put. I put it as a Wetland Activity type and said in the comments “2008 hydroseeding 1.5 acres”</t>
   </si>
   <si>
     <t>Fredrickson Wetland Project (WRP - Palouse Slough)</t>
@@ -876,8 +879,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L14" activeCellId="0" pane="topLeft" sqref="L14"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K16" activeCellId="0" pane="topLeft" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1444,7 +1447,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="195" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="189.55" outlineLevel="0" r="16">
       <c r="A16" s="15" t="n">
         <v>15386</v>
       </c>
@@ -1477,6 +1480,9 @@
       </c>
       <c r="K16" s="16" t="s">
         <v>105</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="17">
@@ -1487,10 +1493,10 @@
         <v>20120429</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>12</v>
@@ -1499,10 +1505,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>24</v>
@@ -1511,7 +1517,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
@@ -1522,22 +1528,22 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
@@ -1546,7 +1552,7 @@
         <v>99</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1557,10 +1563,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1569,10 +1575,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>13</v>
@@ -1581,7 +1587,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1592,10 +1598,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1604,10 +1610,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>13</v>
@@ -1616,7 +1622,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1627,22 +1633,22 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
@@ -1651,7 +1657,7 @@
         <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15387 fixed by gingers comments
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>project_id</t>
   </si>
@@ -437,8 +437,7 @@
     <t>Curry,Josephine,Douglas</t>
   </si>
   <si>
-    <t>These points appear to be misidentified as belonging to project 20120257, ri # 15297 instead of 201020272, 15272
- </t>
+    <t>These points appear to be misidentified as belonging to project 20120257, ri # 15297 instead of 201020272, 15272</t>
   </si>
   <si>
     <t>OK, fixed.</t>
@@ -502,6 +501,9 @@
   </si>
   <si>
     <t>Roughly the same comments as 15386 above.  Remove all of the individual points.  The wetland info (improvement and vegetation planting) should be a polygon following the maroon outline in the respondent map. The only line features required  to capture all the instream and riparian  work would be object ID 83 (fencing) and object ID 86.</t>
+  </si>
+  <si>
+    <t>Done.</t>
   </si>
   <si>
     <t>Eight-Mile Creek Culvert Replacement</t>
@@ -559,7 +561,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -654,12 +656,6 @@
       <b val="true"/>
       <sz val="11"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="11"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -734,31 +730,31 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="21">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="20">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -778,23 +774,23 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="12" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="12" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -806,8 +802,8 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="TableStyleLight1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in TableStyleLight1" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -879,8 +875,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K16" activeCellId="0" pane="topLeft" sqref="K16"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L17" activeCellId="0" pane="topLeft" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1519,6 +1515,9 @@
       <c r="K17" s="16" t="s">
         <v>111</v>
       </c>
+      <c r="L17" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
       <c r="A18" s="12" t="n">
@@ -1528,22 +1527,22 @@
         <v>20120366</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>16</v>
@@ -1552,7 +1551,7 @@
         <v>99</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
@@ -1563,10 +1562,10 @@
         <v>20120431</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>12</v>
@@ -1587,7 +1586,7 @@
         <v>17</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
@@ -1598,10 +1597,10 @@
         <v>20120432</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>12</v>
@@ -1622,7 +1621,7 @@
         <v>17</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
@@ -1633,22 +1632,22 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
@@ -1657,7 +1656,7 @@
         <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished going through gingers comments
</commit_message>
<xml_diff>
--- a/notes/ginger-comments-2013-07-23.xlsx
+++ b/notes/ginger-comments-2013-07-23.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="130">
   <si>
     <t>project_id</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>Haynes Way Fish Passage Improvements- Site 4</t>
+  </si>
+  <si>
+    <t>Done. I'm curious, how did you catch this one? It's quite close to the intersection of road and stream, but not exactly.</t>
   </si>
   <si>
     <t>Willow Creek Bench Tailwater Recovery</t>
@@ -802,8 +805,8 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in TableStyleLight1" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in TableStyleLight1" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -875,8 +878,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L17" activeCellId="0" pane="topLeft" sqref="L17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A17" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L21" activeCellId="0" pane="topLeft" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1553,6 +1556,9 @@
       <c r="K18" s="13" t="s">
         <v>118</v>
       </c>
+      <c r="L18" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="19">
       <c r="A19" s="15" t="n">
@@ -1588,6 +1594,9 @@
       <c r="K19" s="13" t="s">
         <v>121</v>
       </c>
+      <c r="L19" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="20">
       <c r="A20" s="15" t="n">
@@ -1623,6 +1632,9 @@
       <c r="K20" s="13" t="s">
         <v>121</v>
       </c>
+      <c r="L20" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="60" outlineLevel="0" r="21">
       <c r="A21" s="12" t="n">
@@ -1632,22 +1644,22 @@
         <v>20120464</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I21" s="12" t="n">
         <v>27</v>
@@ -1656,7 +1668,10 @@
         <v>67</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>